<commit_message>
satya code for payment and reusable components
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/TestRunner.xlsx
+++ b/src/test/resources/excel/TestRunner.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pawasthi008\Documents\Automation\DemoAutomation\TestAutomation_DemoInstance\src\test\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PwCUIDemo\DemoInstanceAutomation\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8025F99-C1E0-4F58-A4F7-363BB88402C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D642B262-9002-48C4-B3B8-CB8F166E4DC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Run_Manager" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="326">
   <si>
     <t>TestName</t>
   </si>
@@ -985,6 +985,27 @@
   </si>
   <si>
     <t xml:space="preserve">Payment </t>
+  </si>
+  <si>
+    <t>Payment</t>
+  </si>
+  <si>
+    <t>verifyPaymentInformationPageObjects</t>
+  </si>
+  <si>
+    <t>verifyBankPaymentFormFields</t>
+  </si>
+  <si>
+    <t>to verify payment information page objects</t>
+  </si>
+  <si>
+    <t>verify bank payment form fields</t>
+  </si>
+  <si>
+    <t>verifyBankPaymentFormFieldsValidation</t>
+  </si>
+  <si>
+    <t>validation on bank payment form</t>
   </si>
 </sst>
 </file>
@@ -1330,22 +1351,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F110"/>
+  <dimension ref="A1:F113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A98" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C113" sqref="C113"/>
+    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C116" sqref="C116"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.90625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="86.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.90625" style="2"/>
-    <col min="7" max="16384" width="8.90625" style="1"/>
+    <col min="1" max="1" width="21.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="86.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.88671875" style="2"/>
+    <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -1365,7 +1386,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -1385,7 +1406,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -1405,7 +1426,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -1425,7 +1446,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -1445,7 +1466,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -1465,7 +1486,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -1485,7 +1506,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -1505,7 +1526,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -1525,7 +1546,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
@@ -1545,7 +1566,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
@@ -1565,7 +1586,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>7</v>
       </c>
@@ -1585,7 +1606,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>7</v>
       </c>
@@ -1605,7 +1626,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>7</v>
       </c>
@@ -1625,7 +1646,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>9</v>
       </c>
@@ -1645,7 +1666,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>9</v>
       </c>
@@ -1665,7 +1686,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>9</v>
       </c>
@@ -1685,7 +1706,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>9</v>
       </c>
@@ -1705,7 +1726,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>14</v>
       </c>
@@ -1725,7 +1746,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>16</v>
       </c>
@@ -1745,7 +1766,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>68</v>
       </c>
@@ -1765,7 +1786,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>68</v>
       </c>
@@ -1785,7 +1806,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>68</v>
       </c>
@@ -1805,7 +1826,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>68</v>
       </c>
@@ -1825,7 +1846,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>68</v>
       </c>
@@ -1845,7 +1866,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>68</v>
       </c>
@@ -1865,7 +1886,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>68</v>
       </c>
@@ -1885,7 +1906,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>68</v>
       </c>
@@ -1905,7 +1926,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>68</v>
       </c>
@@ -1925,7 +1946,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>93</v>
       </c>
@@ -1945,7 +1966,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>93</v>
       </c>
@@ -1965,7 +1986,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>93</v>
       </c>
@@ -1985,7 +2006,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>93</v>
       </c>
@@ -2005,7 +2026,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>93</v>
       </c>
@@ -2025,7 +2046,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>93</v>
       </c>
@@ -2045,7 +2066,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>93</v>
       </c>
@@ -2065,7 +2086,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>93</v>
       </c>
@@ -2085,7 +2106,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>93</v>
       </c>
@@ -2105,7 +2126,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>93</v>
       </c>
@@ -2125,7 +2146,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>93</v>
       </c>
@@ -2145,7 +2166,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>93</v>
       </c>
@@ -2165,7 +2186,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>93</v>
       </c>
@@ -2185,7 +2206,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>93</v>
       </c>
@@ -2205,7 +2226,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>93</v>
       </c>
@@ -2225,7 +2246,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>93</v>
       </c>
@@ -2245,7 +2266,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>93</v>
       </c>
@@ -2265,7 +2286,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>93</v>
       </c>
@@ -2285,7 +2306,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>93</v>
       </c>
@@ -2305,7 +2326,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>93</v>
       </c>
@@ -2325,7 +2346,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>93</v>
       </c>
@@ -2345,7 +2366,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>93</v>
       </c>
@@ -2365,7 +2386,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>93</v>
       </c>
@@ -2385,7 +2406,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>93</v>
       </c>
@@ -2405,7 +2426,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>93</v>
       </c>
@@ -2425,7 +2446,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>93</v>
       </c>
@@ -2445,7 +2466,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>93</v>
       </c>
@@ -2465,7 +2486,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>93</v>
       </c>
@@ -2485,7 +2506,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>93</v>
       </c>
@@ -2505,7 +2526,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>93</v>
       </c>
@@ -2525,7 +2546,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>93</v>
       </c>
@@ -2545,7 +2566,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>93</v>
       </c>
@@ -2565,7 +2586,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>93</v>
       </c>
@@ -2585,7 +2606,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>93</v>
       </c>
@@ -2605,7 +2626,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>191</v>
       </c>
@@ -2625,7 +2646,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>191</v>
       </c>
@@ -2645,7 +2666,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>191</v>
       </c>
@@ -2665,7 +2686,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>191</v>
       </c>
@@ -2685,7 +2706,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>191</v>
       </c>
@@ -2705,7 +2726,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>191</v>
       </c>
@@ -2725,7 +2746,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>191</v>
       </c>
@@ -2745,7 +2766,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>191</v>
       </c>
@@ -2765,7 +2786,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>191</v>
       </c>
@@ -2785,7 +2806,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>191</v>
       </c>
@@ -2805,7 +2826,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>191</v>
       </c>
@@ -2825,7 +2846,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>191</v>
       </c>
@@ -2845,7 +2866,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>191</v>
       </c>
@@ -2865,7 +2886,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>191</v>
       </c>
@@ -2885,7 +2906,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>191</v>
       </c>
@@ -2905,7 +2926,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>191</v>
       </c>
@@ -2925,7 +2946,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>191</v>
       </c>
@@ -2945,7 +2966,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>191</v>
       </c>
@@ -2965,7 +2986,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>191</v>
       </c>
@@ -2985,7 +3006,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>191</v>
       </c>
@@ -3005,7 +3026,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>252</v>
       </c>
@@ -3025,7 +3046,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>252</v>
       </c>
@@ -3045,7 +3066,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>258</v>
       </c>
@@ -3065,7 +3086,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>258</v>
       </c>
@@ -3085,7 +3106,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>258</v>
       </c>
@@ -3105,7 +3126,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>265</v>
       </c>
@@ -3125,7 +3146,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>271</v>
       </c>
@@ -3145,7 +3166,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>271</v>
       </c>
@@ -3165,7 +3186,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>271</v>
       </c>
@@ -3185,7 +3206,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>7</v>
       </c>
@@ -3205,7 +3226,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>7</v>
       </c>
@@ -3225,7 +3246,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>7</v>
       </c>
@@ -3245,7 +3266,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>281</v>
       </c>
@@ -3265,7 +3286,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>284</v>
       </c>
@@ -3285,7 +3306,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>287</v>
       </c>
@@ -3305,7 +3326,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>287</v>
       </c>
@@ -3325,7 +3346,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>287</v>
       </c>
@@ -3345,7 +3366,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>287</v>
       </c>
@@ -3365,7 +3386,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>7</v>
       </c>
@@ -3385,7 +3406,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>7</v>
       </c>
@@ -3405,7 +3426,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>7</v>
       </c>
@@ -3425,7 +3446,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>7</v>
       </c>
@@ -3445,7 +3466,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>302</v>
       </c>
@@ -3465,7 +3486,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>307</v>
       </c>
@@ -3485,7 +3506,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>310</v>
       </c>
@@ -3505,7 +3526,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>314</v>
       </c>
@@ -3525,7 +3546,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>318</v>
       </c>
@@ -3536,12 +3557,72 @@
         <v>317</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>257</v>
+        <v>18</v>
       </c>
       <c r="E110" s="3" t="s">
         <v>274</v>
       </c>
       <c r="F110" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A111" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="D111" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E111" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F111" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A112" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="D112" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E112" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F112" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A113" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="D113" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="E113" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F113" s="3" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>